<commit_message>
Added Snapshot, Leaderboard and Score Tracker
</commit_message>
<xml_diff>
--- a/Server/Data/schedule.xlsx
+++ b/Server/Data/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KING/Desktop/GitHub/GolfProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3305FCB-99A0-5946-B56B-B9851230645B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B19909-43A9-BF4C-ADB0-1D0DBB710B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{69E209EB-5B8A-FF41-8B56-07AD1F4FF268}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{69E209EB-5B8A-FF41-8B56-07AD1F4FF268}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>THE PLAYERS Championship</t>
   </si>
@@ -113,13 +113,7 @@
     <t>Selection</t>
   </si>
   <si>
-    <t xml:space="preserve">Arnold Palmer Invitational </t>
-  </si>
-  <si>
     <t xml:space="preserve">the Memorial Tournament </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cognizant Classic </t>
   </si>
   <si>
     <t xml:space="preserve">Purse </t>
@@ -129,9 +123,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -181,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -189,13 +180,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -536,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5B841F-4FE1-6848-94FE-7C2AA9C1EC24}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -557,311 +542,290 @@
         <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>45715</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="7">
-        <v>9200000</v>
+      <c r="A2" s="4">
+        <v>45729</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5">
+        <v>25000000</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>45722</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="4">
+        <v>45736</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <v>8700000</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>45743</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>9500000</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>45750</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <v>9500000</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>45757</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>45764</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>45778</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <v>9900000</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>45785</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>45792</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>45799</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
+        <v>9500000</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>45806</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="7">
-        <v>20000000</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="6">
-        <v>45729</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="7">
-        <v>25000000</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
-        <v>45736</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7">
-        <v>8700000</v>
-      </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>45743</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7">
-        <v>9500000</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>45750</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7">
-        <v>9500000</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>45757</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="7">
-        <v>20000000</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>45764</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="7">
-        <v>20000000</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>45778</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="7">
-        <v>9900000</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
-        <v>45785</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="7">
-        <v>20000000</v>
-      </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
-        <v>45792</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="C12" s="5">
         <v>20000000</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>45799</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="7">
-        <v>9500000</v>
+      <c r="A13" s="4">
+        <v>45813</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="5">
+        <v>9800000</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6">
-        <v>45806</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="A14" s="4">
+        <v>45820</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="5">
         <v>20000000</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6">
-        <v>45813</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="7">
-        <v>9800000</v>
+      <c r="A15" s="4">
+        <v>45827</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="5">
+        <v>20000000</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6">
-        <v>45820</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="7">
-        <v>20000000</v>
+      <c r="A16" s="4">
+        <v>45834</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="5">
+        <v>9600000</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="6">
-        <v>45827</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="7">
-        <v>20000000</v>
+      <c r="A17" s="4">
+        <v>45841</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="5">
+        <v>8400000</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
-        <v>45834</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="7">
-        <v>9600000</v>
+      <c r="A18" s="4">
+        <v>45848</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5">
+        <v>9000000</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="6">
-        <v>45841</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="A19" s="4">
+        <v>45855</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>45862</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="5">
         <v>8400000</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="6">
-        <v>45848</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="7">
-        <v>9000000</v>
-      </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="6">
-        <v>45855</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="7">
-        <v>20000000</v>
+      <c r="A21" s="4">
+        <v>45869</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="5">
+        <v>8200000</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="6">
-        <v>45862</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7">
-        <v>8400000</v>
+      <c r="A22" s="4">
+        <v>45876</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5">
+        <v>20000000</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="6">
-        <v>45869</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="7">
-        <v>8200000</v>
+      <c r="A23" s="4">
+        <v>45883</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="5">
+        <v>20000000</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
-        <v>45876</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="7">
+      <c r="A24" s="4">
+        <v>45890</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="5">
         <v>20000000</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6">
-        <v>45883</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="7">
-        <v>20000000</v>
-      </c>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6">
-        <v>45890</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="7">
-        <v>20000000</v>
-      </c>
-      <c r="D26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Enhanced Score Tracker UI and functionality: - Modified table height to show 5 rows - Increased row height and spacing - Made event names bolder - Fixed numeric column types in database - Added result processing from Excel file
</commit_message>
<xml_diff>
--- a/Server/Data/schedule.xlsx
+++ b/Server/Data/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KING/Desktop/GitHub/GolfProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KING/Desktop/GitHub/GolfProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B19909-43A9-BF4C-ADB0-1D0DBB710B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BE6998-2390-6C40-B686-BB65FB2CCC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{69E209EB-5B8A-FF41-8B56-07AD1F4FF268}"/>
   </bookViews>
@@ -113,10 +113,10 @@
     <t>Selection</t>
   </si>
   <si>
-    <t xml:space="preserve">the Memorial Tournament </t>
-  </si>
-  <si>
     <t xml:space="preserve">Purse </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Memorial Tournament </t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,7 +542,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>24</v>
@@ -562,7 +562,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>45736</v>
+        <v>45738</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -673,7 +673,7 @@
         <v>45806</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5">
         <v>20000000</v>

</xml_diff>

<commit_message>
Add user authentication: Registration page, navigation updates, and database schema changes for user management
</commit_message>
<xml_diff>
--- a/Server/Data/schedule.xlsx
+++ b/Server/Data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KING/Desktop/GitHub/GolfProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BE6998-2390-6C40-B686-BB65FB2CCC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A9ECCF-92C9-3A46-8756-E560C53A76A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{69E209EB-5B8A-FF41-8B56-07AD1F4FF268}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>THE PLAYERS Championship</t>
-  </si>
-  <si>
-    <t>Valspar Championship</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Texas Children's Houston Open</t>
   </si>
@@ -521,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5B841F-4FE1-6848-94FE-7C2AA9C1EC24}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,81 +530,81 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>45729</v>
+        <v>45743</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="5">
-        <v>25000000</v>
+        <v>9500000</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>45738</v>
+        <v>45750</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5">
-        <v>8700000</v>
+        <v>9500000</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>45743</v>
+        <v>45757</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="5">
-        <v>9500000</v>
+        <v>20000000</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>45750</v>
+        <v>45764</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5">
-        <v>9500000</v>
+        <v>20000000</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
-        <v>45757</v>
+        <v>45778</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="5">
-        <v>20000000</v>
+        <v>9900000</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
-        <v>45764</v>
+        <v>45785</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -622,34 +616,34 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
-        <v>45778</v>
+        <v>45792</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="5">
-        <v>9900000</v>
+        <v>20000000</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
-        <v>45785</v>
+        <v>45799</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5">
-        <v>20000000</v>
+        <v>9500000</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
-        <v>45792</v>
+        <v>45806</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C10" s="5">
         <v>20000000</v>
@@ -658,22 +652,22 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
-        <v>45799</v>
+        <v>45813</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="5">
-        <v>9500000</v>
+        <v>9800000</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
-        <v>45806</v>
+        <v>45820</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C12" s="5">
         <v>20000000</v>
@@ -682,115 +676,115 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
-        <v>45813</v>
+        <v>45827</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="5">
-        <v>9800000</v>
+        <v>20000000</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
-        <v>45820</v>
+        <v>45834</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="5">
-        <v>20000000</v>
+        <v>9600000</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
-        <v>45827</v>
+        <v>45841</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="5">
-        <v>20000000</v>
+        <v>8400000</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="5">
-        <v>9600000</v>
+        <v>9000000</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
-        <v>45841</v>
-      </c>
-      <c r="B17" s="3" t="s">
+        <v>45855</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="5">
-        <v>8400000</v>
+        <v>20000000</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
-        <v>45848</v>
+        <v>45862</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="5">
-        <v>9000000</v>
+        <v>8400000</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
-        <v>45855</v>
-      </c>
-      <c r="B19" s="2" t="s">
+        <v>45869</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="5">
-        <v>20000000</v>
+        <v>8200000</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
-        <v>45862</v>
+        <v>45876</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="5">
-        <v>8400000</v>
+        <v>20000000</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
-        <v>45869</v>
+        <v>45883</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="5">
-        <v>8200000</v>
+        <v>20000000</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
-        <v>45876</v>
+        <v>45890</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>19</v>
@@ -801,31 +795,7 @@
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>45883</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="5">
-        <v>20000000</v>
-      </c>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>45890</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="5">
-        <v>20000000</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed score tracker and user-specific data handling: - Updated unique constraints to allow multiple users per event - Fixed tournament selection locking - Added proper user authentication - Improved frontend display of user-specific data
</commit_message>
<xml_diff>
--- a/Server/Data/schedule.xlsx
+++ b/Server/Data/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KING/Desktop/GitHub/GolfProject/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A9ECCF-92C9-3A46-8756-E560C53A76A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA247B9A-708B-0B40-A5FB-9D8611C5792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{69E209EB-5B8A-FF41-8B56-07AD1F4FF268}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{69E209EB-5B8A-FF41-8B56-07AD1F4FF268}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>45743</v>
+        <v>45746</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>

</xml_diff>